<commit_message>
use tiger/line geography abbreviations
make accepted abbreviations for geography() option consistent with [TIGER/Line](https://www2.census.gov/geo/tiger/TIGER2020/2020_TL_Shapefiles_File_Name_Definitions.pdf).
plus a small fix: only 5-year estimates are available for state legislative districts
</commit_message>
<xml_diff>
--- a/dev/getcensus_geo_args.xlsx
+++ b/dev/getcensus_geo_args.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\getcensus\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513C8F0-51AA-45DA-97C6-F6F4652845F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F791A-1229-407A-86ED-2A7F74DA2182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="313" yWindow="207" windowWidth="13860" windowHeight="8533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="313" yWindow="187" windowWidth="13860" windowHeight="8533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t/>
   </si>
   <si>
-    <t>ancsa</t>
-  </si>
-  <si>
     <t>metro</t>
   </si>
   <si>
@@ -145,37 +142,40 @@
     <t>cd</t>
   </si>
   <si>
-    <t>sche</t>
-  </si>
-  <si>
-    <t>schs</t>
-  </si>
-  <si>
-    <t>sch</t>
-  </si>
-  <si>
     <t>puma</t>
   </si>
   <si>
     <t>zcta</t>
   </si>
   <si>
-    <t>slupper</t>
-  </si>
-  <si>
-    <t>sllower</t>
-  </si>
-  <si>
     <t>state county</t>
   </si>
   <si>
     <t>geo_hierarchy</t>
   </si>
   <si>
-    <t>aiaanahhl</t>
-  </si>
-  <si>
     <t>co</t>
+  </si>
+  <si>
+    <t>sldu</t>
+  </si>
+  <si>
+    <t>sldl</t>
+  </si>
+  <si>
+    <t>elsd</t>
+  </si>
+  <si>
+    <t>unsd</t>
+  </si>
+  <si>
+    <t>scsd</t>
+  </si>
+  <si>
+    <t>anrc</t>
+  </si>
+  <si>
+    <t>aiannh</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -549,7 +549,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -603,7 +603,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -614,7 +614,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -625,7 +625,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -655,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -687,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -695,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -703,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -714,7 +714,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -725,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -736,7 +736,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -747,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -758,7 +758,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -777,7 +777,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
various fixes to geography error checks
fix #42
fix #39
corrections to which geographies may be combined with statefips()
check sample is available for geography before other checks

Update getcensus.ado
</commit_message>
<xml_diff>
--- a/dev/getcensus_geo_args.xlsx
+++ b/dev/getcensus_geo_args.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\getcensus\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F791A-1229-407A-86ED-2A7F74DA2182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B15A1E-3B35-4C37-AF49-46E82E92C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="313" yWindow="187" windowWidth="13860" windowHeight="8533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>geo_names</t>
   </si>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -760,6 +760,9 @@
       <c r="B23" t="s">
         <v>41</v>
       </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">

</xml_diff>

<commit_message>
Revert "Merge branch 'version-2' of https://github.com/CenterOnBudget/getcensus into version-2"
This reverts commit 21341f64fa8c0cd118a82084478d4ca43e71e1de, reversing
changes made to ec0bf146cd04e18748c5fff0d1c762371e7459fc.
</commit_message>
<xml_diff>
--- a/dev/getcensus_geo_args.xlsx
+++ b/dev/getcensus_geo_args.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\getcensus\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B15A1E-3B35-4C37-AF49-46E82E92C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F13138-8C24-46C7-B946-E8D9F01275EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="313" yWindow="187" windowWidth="13860" windowHeight="8533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="393" yWindow="0" windowWidth="15154" windowHeight="8133" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>geo_names</t>
   </si>
@@ -112,6 +112,9 @@
     <t/>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>cousub</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t/>
   </si>
   <si>
+    <t>ancsa</t>
+  </si>
+  <si>
     <t>metro</t>
   </si>
   <si>
@@ -142,40 +148,34 @@
     <t>cd</t>
   </si>
   <si>
+    <t>sche</t>
+  </si>
+  <si>
+    <t>schs</t>
+  </si>
+  <si>
+    <t>sch</t>
+  </si>
+  <si>
     <t>puma</t>
   </si>
   <si>
     <t>zcta</t>
   </si>
   <si>
+    <t>slupper</t>
+  </si>
+  <si>
+    <t>sllower</t>
+  </si>
+  <si>
     <t>state county</t>
   </si>
   <si>
     <t>geo_hierarchy</t>
   </si>
   <si>
-    <t>co</t>
-  </si>
-  <si>
-    <t>sldu</t>
-  </si>
-  <si>
-    <t>sldl</t>
-  </si>
-  <si>
-    <t>elsd</t>
-  </si>
-  <si>
-    <t>unsd</t>
-  </si>
-  <si>
-    <t>scsd</t>
-  </si>
-  <si>
-    <t>anrc</t>
-  </si>
-  <si>
-    <t>aiannh</t>
+    <t>aiaanahhl</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -549,7 +549,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -600,10 +600,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -611,10 +611,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -622,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -633,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -687,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -695,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -703,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -714,7 +714,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -725,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -736,7 +736,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -747,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -758,10 +758,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -769,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -780,7 +777,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
revert to commit 4fab33f
https://github.com/CenterOnBudget/getcensus/commit/4fab33f497ddb4a03baa40a5f44920f8e7fcb107
</commit_message>
<xml_diff>
--- a/dev/getcensus_geo_args.xlsx
+++ b/dev/getcensus_geo_args.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\czippel\Documents\GitHub\getcensus\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F13138-8C24-46C7-B946-E8D9F01275EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B15A1E-3B35-4C37-AF49-46E82E92C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="393" yWindow="0" windowWidth="15154" windowHeight="8133" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="313" yWindow="187" windowWidth="13860" windowHeight="8533" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>geo_names</t>
   </si>
@@ -112,24 +112,18 @@
     <t/>
   </si>
   <si>
+    <t>cousub</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>cousub</t>
+    <t>bg</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>bg</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ancsa</t>
-  </si>
-  <si>
     <t>metro</t>
   </si>
   <si>
@@ -148,34 +142,40 @@
     <t>cd</t>
   </si>
   <si>
-    <t>sche</t>
-  </si>
-  <si>
-    <t>schs</t>
-  </si>
-  <si>
-    <t>sch</t>
-  </si>
-  <si>
     <t>puma</t>
   </si>
   <si>
     <t>zcta</t>
   </si>
   <si>
-    <t>slupper</t>
-  </si>
-  <si>
-    <t>sllower</t>
-  </si>
-  <si>
     <t>state county</t>
   </si>
   <si>
     <t>geo_hierarchy</t>
   </si>
   <si>
-    <t>aiaanahhl</t>
+    <t>co</t>
+  </si>
+  <si>
+    <t>sldu</t>
+  </si>
+  <si>
+    <t>sldl</t>
+  </si>
+  <si>
+    <t>elsd</t>
+  </si>
+  <si>
+    <t>unsd</t>
+  </si>
+  <si>
+    <t>scsd</t>
+  </si>
+  <si>
+    <t>anrc</t>
+  </si>
+  <si>
+    <t>aiannh</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -549,7 +549,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -589,7 +589,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -600,10 +600,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -611,10 +611,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -622,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -633,7 +633,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -663,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -687,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -695,7 +695,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -703,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -714,7 +714,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -725,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>4</v>
@@ -736,7 +736,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -747,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -758,7 +758,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -766,7 +769,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>4</v>
@@ -777,7 +780,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>4</v>

</xml_diff>